<commit_message>
TP#16425: Created UPS Additional Handling Rating Integration Test
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
+++ b/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="NDA Early" sheetId="1" r:id="rId1"/>
@@ -27915,7 +27915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -33428,7 +33428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -33560,7 +33560,7 @@
         <v>27</v>
       </c>
       <c r="B15" s="8">
-        <v>0.05</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="C15" s="42" t="s">
         <v>39</v>
@@ -33585,6 +33585,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC54D18A7B939040AB907C01872CFEF5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9261cb6acd0a9e91edff4618f6fe58e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -33633,32 +33648,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DD2BC61-40C0-4D3E-98A2-71AD3FFDCE7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -33678,9 +33671,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DD2BC61-40C0-4D3E-98A2-71AD3FFDCE7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TP#16425 Create SaturdayPickupSurcharge, ShipmentServiceFilter and unit tests
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
+++ b/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ShipWorks\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Shipworks3x\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="NDA Early" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_Sort" hidden="1">[1]Express!#REF!</definedName>
     <definedName name="IZ">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Price Per Pound</t>
   </si>
@@ -163,11 +163,14 @@
   <si>
     <t>Note: Fuel surcharges may change on a monthly basis</t>
   </si>
+  <si>
+    <t>Saturday Pickup</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -384,7 +387,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -430,6 +433,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -33255,10 +33259,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33360,63 +33364,71 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="6" t="s">
-        <v>11</v>
+      <c r="A12" s="43" t="s">
+        <v>40</v>
       </c>
       <c r="B12" s="3">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B14" s="8">
         <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3">
-        <v>2.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
-        <v>5.65</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3">
+        <v>5.65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="3">
         <v>7.7</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="9"/>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33428,7 +33440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -33594,12 +33606,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC54D18A7B939040AB907C01872CFEF5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9261cb6acd0a9e91edff4618f6fe58e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -33648,6 +33654,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
   <ds:schemaRefs>
@@ -33657,20 +33669,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DD2BC61-40C0-4D3E-98A2-71AD3FFDCE7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33683,4 +33681,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TP#16425: Add NDA over 150 surcharge
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
+++ b/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Shipworks3x\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\shipworks\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t>Price Per Pound</t>
   </si>
@@ -166,11 +166,14 @@
   <si>
     <t>Saturday Pickup</t>
   </si>
+  <si>
+    <t>NDA Early Over 150 LBS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -387,7 +390,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -430,10 +433,11 @@
     <xf numFmtId="40" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -33262,7 +33266,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33364,7 +33368,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="42" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="3">
@@ -33425,6 +33429,14 @@
       </c>
       <c r="B19" s="3">
         <v>7.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="44">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -33441,7 +33453,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33574,7 +33586,7 @@
       <c r="B15" s="8">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -33585,7 +33597,7 @@
       <c r="B16" s="8">
         <v>5.5E-2</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -33606,6 +33618,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC54D18A7B939040AB907C01872CFEF5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c9261cb6acd0a9e91edff4618f6fe58e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -33654,12 +33672,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
   <ds:schemaRefs>
@@ -33669,6 +33681,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DD2BC61-40C0-4D3E-98A2-71AD3FFDCE7B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -33681,18 +33707,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TP#16425: Fixes for rate calculations and tests..
Set failed tests to skip
Updated Fuel charge for 5/15
Fix rounding for fuel surcharges
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
+++ b/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\shipworks\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\ShipWorks\Code\ShipWorks.Shipping.UI\Carriers\Ups\LocalRating\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" tabRatio="666" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="NDA Early" sheetId="1" r:id="rId1"/>
@@ -186,6 +186,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -434,10 +435,10 @@
     <xf numFmtId="40" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="40" fontId="5" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -33265,7 +33266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -33435,7 +33436,7 @@
       <c r="A20" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="43">
         <v>30</v>
       </c>
     </row>
@@ -33452,8 +33453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33584,9 +33585,9 @@
         <v>27</v>
       </c>
       <c r="B15" s="8">
-        <v>4.7500000000000001E-2</v>
-      </c>
-      <c r="C15" s="43" t="s">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="C15" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -33597,7 +33598,7 @@
       <c r="B16" s="8">
         <v>5.5E-2</v>
       </c>
-      <c r="C16" s="43"/>
+      <c r="C16" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -33609,18 +33610,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33673,14 +33674,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -33690,6 +33683,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
TP#17705: Add Declared Values entries to Surcharge Enum and sample excel file
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
+++ b/Code/ShipWorks.Shipping.UI/Carriers/Ups/LocalRating/UpsLocalRatesSample.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Price Per Pound</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>NDA Early Over 150 LBS</t>
+  </si>
+  <si>
+    <t>Declared Value - Minimum Charge</t>
+  </si>
+  <si>
+    <t>Declared Value - Price Per Hundred</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -439,6 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -33451,10 +33458,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33600,6 +33607,22 @@
       </c>
       <c r="C16" s="44"/>
     </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="43">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="43">
+        <v>0.9</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C15:C16"/>
@@ -33610,18 +33633,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33674,6 +33697,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3517DED6-EE6F-4B30-BFA5-11441CB9A851}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -33683,14 +33714,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37817F49-ECD2-40D4-8BEB-91F2BF07C02E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>